<commit_message>
Manage Page : Added Logic for fetching and filtering and sorting , Excel based Insertion , Pagination
</commit_message>
<xml_diff>
--- a/frontend/public/templates/MarcheTemplate.xlsx
+++ b/frontend/public/templates/MarcheTemplate.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\school\Stage\Projet\frontend\public\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lenovo\Desktop\school\Stage\Projet de Gestion des materiels informatiques\Source code\frontend\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -41,10 +41,10 @@
     <t>Date de Creation</t>
   </si>
   <si>
-    <t>**/**</t>
-  </si>
-  <si>
-    <t>DD-MM-YYYY</t>
+    <t>YYYY-MM-DD</t>
+  </si>
+  <si>
+    <t>****/**</t>
   </si>
 </sst>
 </file>
@@ -366,7 +366,7 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -395,10 +395,10 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>